<commit_message>
added some slides for ch2 and ch3, ch3 is still WIP
</commit_message>
<xml_diff>
--- a/doc/Translation file to Spanish.xlsx
+++ b/doc/Translation file to Spanish.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28410"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotoo2920\Documents\GitHub\node_dev\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.orta.santana/Github/node_dev/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13185"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
     <sheet name="Español" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>Index Page</t>
   </si>
@@ -106,12 +112,252 @@
   </si>
   <si>
     <t>Chaper 1</t>
+  </si>
+  <si>
+    <t>What is Diabetes?</t>
+  </si>
+  <si>
+    <t>ch1-0</t>
+  </si>
+  <si>
+    <t>ch1-1</t>
+  </si>
+  <si>
+    <t>ch1-2</t>
+  </si>
+  <si>
+    <t>ch1-3</t>
+  </si>
+  <si>
+    <t>ch1-4</t>
+  </si>
+  <si>
+    <t>ch1-5</t>
+  </si>
+  <si>
+    <t>ch1-6</t>
+  </si>
+  <si>
+    <t>ch1-7</t>
+  </si>
+  <si>
+    <t>ch1-8</t>
+  </si>
+  <si>
+    <t>ch1-9</t>
+  </si>
+  <si>
+    <t>ch1-10</t>
+  </si>
+  <si>
+    <t>ch1-11</t>
+  </si>
+  <si>
+    <t>ch1-12</t>
+  </si>
+  <si>
+    <t>Chapter 1</t>
+  </si>
+  <si>
+    <t>Animation 1.1 What is Diabetes?</t>
+  </si>
+  <si>
+    <t>Let’s Review</t>
+  </si>
+  <si>
+    <t>There are two main types of diabetes</t>
+  </si>
+  <si>
+    <t>The part of the body that makes insulin</t>
+  </si>
+  <si>
+    <t>Type 1 diabetes happens when the body is not able to make enough insulin in the pancreas</t>
+  </si>
+  <si>
+    <t>A hormone that lowers blood glucose levels</t>
+  </si>
+  <si>
+    <t>Type 2 diabetes happens when the body cannot use insulin correctly</t>
+  </si>
+  <si>
+    <t>What is insulin and why is it so important?</t>
+  </si>
+  <si>
+    <t>Insulin is needed to move glucose from the blood into cells in the body that use it for energy</t>
+  </si>
+  <si>
+    <t>Major source of energy for the body’s cells. It mainly comes from the foods we eat</t>
+  </si>
+  <si>
+    <t>Type 2 diabetes happens when the body cannot use insulin correctly</t>
+  </si>
+  <si>
+    <t>ch1-13</t>
+  </si>
+  <si>
+    <t>ch1-14</t>
+  </si>
+  <si>
+    <t>ch1-15</t>
+  </si>
+  <si>
+    <t>ch1-16</t>
+  </si>
+  <si>
+    <t>ch1-17</t>
+  </si>
+  <si>
+    <t>ch1-18</t>
+  </si>
+  <si>
+    <t>ch1-19</t>
+  </si>
+  <si>
+    <t>ch1-20</t>
+  </si>
+  <si>
+    <t>ch1-21</t>
+  </si>
+  <si>
+    <t>ch1-22</t>
+  </si>
+  <si>
+    <t>ch1-23</t>
+  </si>
+  <si>
+    <t>ch1-24</t>
+  </si>
+  <si>
+    <t>ch1-25</t>
+  </si>
+  <si>
+    <t>ch1-26</t>
+  </si>
+  <si>
+    <t>ch1-27</t>
+  </si>
+  <si>
+    <t>Why doesn’t the body make enough insulin in type 1 diabetes?</t>
+  </si>
+  <si>
+    <t>The immune system normally fight infections</t>
+  </si>
+  <si>
+    <t>Attacks</t>
+  </si>
+  <si>
+    <t>Immune System</t>
+  </si>
+  <si>
+    <t>Viruses and bacteria</t>
+  </si>
+  <si>
+    <t>Damaged Viruses and bacteria</t>
+  </si>
+  <si>
+    <t>but</t>
+  </si>
+  <si>
+    <t>In Type 1 diabetes, the immune system attacks the pancreas</t>
+  </si>
+  <si>
+    <t>Pancreas</t>
+  </si>
+  <si>
+    <t>Damaged Pancreas</t>
+  </si>
+  <si>
+    <t>ch1-28</t>
+  </si>
+  <si>
+    <t>ch1-29</t>
+  </si>
+  <si>
+    <t>ch1-30</t>
+  </si>
+  <si>
+    <t>ch1-31</t>
+  </si>
+  <si>
+    <t>ch1-32</t>
+  </si>
+  <si>
+    <t>ch1-33</t>
+  </si>
+  <si>
+    <t>ch1-34</t>
+  </si>
+  <si>
+    <t>ch1-35</t>
+  </si>
+  <si>
+    <t>ch1-36</t>
+  </si>
+  <si>
+    <t>ch1-37</t>
+  </si>
+  <si>
+    <t>ch1-38</t>
+  </si>
+  <si>
+    <t>Low Insulin</t>
+  </si>
+  <si>
+    <t>High Glucose</t>
+  </si>
+  <si>
+    <t>Glucose levels in people without diabetes are usually between 80-100 </t>
+  </si>
+  <si>
+    <t>When there’s not enough insulin, the glucose can go over 200</t>
+  </si>
+  <si>
+    <t>When the glucose is too high it spills into the urine making you go to the bathroom a lot and makes you very thirsty</t>
+  </si>
+  <si>
+    <t>What's up with Ketones?</t>
+  </si>
+  <si>
+    <t>Type 1 diabetes vs. Type 2 diabetes</t>
+  </si>
+  <si>
+    <t>Type 1 diabetes is treated with insulin which is usually given through a needle</t>
+  </si>
+  <si>
+    <t>Type 2 diabetes is sometimes treated with insulin, but usually people can take pills and focus on losing weight</t>
+  </si>
+  <si>
+    <t>What is Insulin ?</t>
+  </si>
+  <si>
+    <t>A. Hormone that lowers glucose levels</t>
+  </si>
+  <si>
+    <t>B. Hormone that raises glucose levels</t>
+  </si>
+  <si>
+    <t>C. Hormone that breaks down fat and protein</t>
+  </si>
+  <si>
+    <t>Please Select one!</t>
+  </si>
+  <si>
+    <t>ch1-39</t>
+  </si>
+  <si>
+    <t>ch1-40</t>
+  </si>
+  <si>
+    <t>Yay!! You are Correct! :)</t>
+  </si>
+  <si>
+    <t>Please Try Again :(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,82 +704,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -549,69 +1123,69 @@
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>